<commit_message>
changes to bce loss and cce loss cupy to prevent nans
</commit_message>
<xml_diff>
--- a/benchmarks_tests/performance-COLAB.xlsx
+++ b/benchmarks_tests/performance-COLAB.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manas\Documents\crysx_nn\benchmarks_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95199F60-D4F2-464D-A804-05ABAC70FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AAD03-DB9F-40F7-9534-2B5D56513726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="1" activeTab="5" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="5" xr2:uid="{F8ACF7B6-A719-5A49-89C3-B4340F0ED991}"/>
   </bookViews>
   <sheets>
     <sheet name="Logic CPU colab" sheetId="1" r:id="rId1"/>
     <sheet name="Logic CPU XPS" sheetId="8" r:id="rId2"/>
     <sheet name="Logic GPU colab" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Logic CPU XPS more layers" sheetId="4" r:id="rId4"/>
     <sheet name="MNIST CPU XPS larger batch size" sheetId="9" r:id="rId5"/>
-    <sheet name="MNIST GPU Colab" sheetId="10" r:id="rId6"/>
-    <sheet name="MNIST CPU XPS" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="MNIST GPU Colab batchsize=40" sheetId="11" r:id="rId6"/>
+    <sheet name="MNIST GPU Colab" sheetId="10" r:id="rId7"/>
+    <sheet name="MNIST CPU XPS" sheetId="5" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
   <si>
     <t>Model</t>
   </si>
@@ -157,9 +158,6 @@
     <t>MNIST Kaggle</t>
   </si>
   <si>
-    <t>num_threads=2</t>
-  </si>
-  <si>
     <t>CrysX-NN (1)</t>
   </si>
   <si>
@@ -173,6 +171,18 @@
   </si>
   <si>
     <t>nepochs=10</t>
+  </si>
+  <si>
+    <t>num_threads=8</t>
+  </si>
+  <si>
+    <t>Tesla K80</t>
+  </si>
+  <si>
+    <t>4000,4000,10</t>
+  </si>
+  <si>
+    <t>batchsize =40</t>
   </si>
 </sst>
 </file>
@@ -261,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -335,6 +345,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1997,19 +2010,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -2026,13 +2033,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Wall</a:t>
+              <a:t>Wall time (s) vs no. of paramaters</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> time (s) vs no. of paramaters</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2049,19 +2051,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -2092,63 +2088,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2184,6 +2144,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2209,63 +2187,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2301,6 +2243,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>46.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2326,63 +2286,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent3">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2418,6 +2342,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2443,63 +2385,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent4">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -2535,6 +2441,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2567,9 +2491,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2584,10 +2508,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -2615,10 +2540,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2638,10 +2564,12 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2652,8 +2580,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2679,9 +2608,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2696,10 +2625,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -2709,7 +2639,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Wall time ()seconds)</a:t>
+                  <a:t>Wall time (seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2727,10 +2657,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2750,10 +2681,12 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2764,8 +2697,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2805,8 +2739,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2830,28 +2765,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2962,7 +2886,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$C$3</c:f>
+              <c:f>'Logic CPU XPS more layers'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3011,7 +2935,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$B$5:$B$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3041,31 +2965,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$C$5:$C$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$C$5:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>19.899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>76</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3081,7 +2984,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$D$3</c:f>
+              <c:f>'Logic CPU XPS more layers'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3130,7 +3033,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$B$5:$B$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3160,31 +3063,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$D$5:$D$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.57</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>71</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3200,7 +3082,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$E$3</c:f>
+              <c:f>'Logic CPU XPS more layers'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3249,7 +3131,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$B$5:$B$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3279,31 +3161,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$E$5:$E$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$E$5:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>37.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3319,7 +3180,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$F$3</c:f>
+              <c:f>'Logic CPU XPS more layers'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3368,7 +3229,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$B$5:$B$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3398,31 +3259,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$F$5:$F$11</c:f>
+              <c:f>'Logic CPU XPS more layers'!$F$5:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>46.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4960,66 +4800,62 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -5028,8 +4864,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5048,6 +4885,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -5056,20 +4901,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -5078,13 +4923,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5096,31 +4941,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5136,18 +4980,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5166,13 +5013,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5184,14 +5032,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -5205,8 +5053,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5220,6 +5069,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -5231,9 +5086,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5248,13 +5103,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -5266,14 +5122,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -5285,13 +5141,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -5300,13 +5157,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -5314,7 +5172,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -5327,34 +5185,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5366,19 +5216,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -5394,7 +5237,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -5403,8 +5246,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5420,13 +5264,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5435,17 +5280,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5457,6 +5305,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -6087,16 +5941,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>763270</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6473,28 +6327,28 @@
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
@@ -6689,28 +6543,28 @@
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="26"/>
@@ -6899,34 +6753,34 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="26"/>
@@ -6939,17 +6793,25 @@
       <c r="B3" s="4">
         <v>261</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" t="e">
+      <c r="C3" s="4">
+        <v>34.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>46.6</v>
+      </c>
+      <c r="E3" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>14</v>
+      </c>
+      <c r="G3">
         <f>E3/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" t="e">
+        <v>0.8492753623188406</v>
+      </c>
+      <c r="H3">
         <f>E3/F3</f>
-        <v>#DIV/0!</v>
+        <v>2.092857142857143</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -6959,17 +6821,25 @@
       <c r="B4" s="6">
         <v>5301</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" t="e">
-        <f t="shared" ref="G4:G8" si="0">E4/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" t="e">
-        <f t="shared" ref="H4:H8" si="1">E4/F4</f>
-        <v>#DIV/0!</v>
+      <c r="C4" s="5">
+        <v>41.2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="E4" s="5">
+        <v>29.3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>12.6</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G5" si="0">E4/C4</f>
+        <v>0.71116504854368934</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H5" si="1">E4/F4</f>
+        <v>2.3253968253968256</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -6979,17 +6849,25 @@
       <c r="B5" s="8">
         <v>20601</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" t="e">
+      <c r="C5" s="7">
+        <v>33.5</v>
+      </c>
+      <c r="D5" s="7">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E5" s="7">
+        <v>29.8</v>
+      </c>
+      <c r="F5" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" t="e">
+        <v>0.88955223880597012</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.3839999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -6999,17 +6877,25 @@
       <c r="B6" s="6">
         <v>503001</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C6" s="5">
+        <v>41.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>40.5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30.3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>12.6</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G8" si="2">E6/C6</f>
+        <v>0.73012048192771084</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H8" si="3">E6/F6</f>
+        <v>2.4047619047619051</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -7019,17 +6905,25 @@
       <c r="B7" s="8">
         <v>2006001</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C7" s="7">
+        <v>41.3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>43.5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>31.8</v>
+      </c>
+      <c r="F7" s="7">
+        <v>13.8</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.76997578692493951</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>2.3043478260869565</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7039,17 +6933,25 @@
       <c r="B8" s="10">
         <v>8012001</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C8" s="9">
+        <v>40.6</v>
+      </c>
+      <c r="D8" s="9">
+        <v>43.4</v>
+      </c>
+      <c r="E8" s="9">
+        <v>32.6</v>
+      </c>
+      <c r="F8" s="9">
+        <v>21.8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.80295566502463056</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>1.4954128440366972</v>
       </c>
     </row>
   </sheetData>
@@ -7067,14 +6969,14 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7083,10 +6985,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -7103,8 +7005,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="2">
         <v>6</v>
       </c>
@@ -7125,25 +7027,17 @@
       <c r="B5" s="13">
         <v>2001</v>
       </c>
-      <c r="C5" s="4">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.57</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.67</v>
-      </c>
-      <c r="G5">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" t="e">
         <f>E5/C5</f>
-        <v>0.1306532663316583</v>
-      </c>
-      <c r="H5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="e">
         <f>E5/F5</f>
-        <v>0.70844686648501365</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
@@ -7153,25 +7047,17 @@
       <c r="B6" s="6">
         <v>252501</v>
       </c>
-      <c r="C6" s="5">
-        <v>39.4</v>
-      </c>
-      <c r="D6" s="5">
-        <v>11.8</v>
-      </c>
-      <c r="E6" s="5">
-        <v>11.6</v>
-      </c>
-      <c r="F6" s="5">
-        <v>10</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" t="e">
         <f t="shared" ref="G6:G11" si="0">E6/C6</f>
-        <v>0.29441624365482233</v>
-      </c>
-      <c r="H6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" t="e">
         <f t="shared" ref="H6:H11" si="1">E6/F6</f>
-        <v>1.1599999999999999</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -7181,25 +7067,17 @@
       <c r="B7" s="8">
         <v>503001</v>
       </c>
-      <c r="C7" s="7">
-        <v>48</v>
-      </c>
-      <c r="D7" s="7">
-        <v>32.6</v>
-      </c>
-      <c r="E7" s="7">
-        <v>29.8</v>
-      </c>
-      <c r="F7" s="7">
-        <v>22.4</v>
-      </c>
-      <c r="G7">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" t="e">
         <f t="shared" si="0"/>
-        <v>0.62083333333333335</v>
-      </c>
-      <c r="H7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
         <f t="shared" si="1"/>
-        <v>1.330357142857143</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -7209,25 +7087,17 @@
       <c r="B8" s="6">
         <v>753501</v>
       </c>
-      <c r="C8" s="5">
-        <v>55.1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>42.8</v>
-      </c>
-      <c r="E8" s="5">
-        <v>37.5</v>
-      </c>
-      <c r="F8" s="5">
-        <v>30.2</v>
-      </c>
-      <c r="G8">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" t="e">
         <f t="shared" si="0"/>
-        <v>0.68058076225045372</v>
-      </c>
-      <c r="H8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" t="e">
         <f t="shared" si="1"/>
-        <v>1.2417218543046358</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="54.9" x14ac:dyDescent="0.6">
@@ -7237,25 +7107,17 @@
       <c r="B9" s="8">
         <v>1004001</v>
       </c>
-      <c r="C9" s="7">
-        <v>67</v>
-      </c>
-      <c r="D9" s="7">
-        <v>51</v>
-      </c>
-      <c r="E9" s="7">
-        <v>43.9</v>
-      </c>
-      <c r="F9" s="7">
-        <v>46.4</v>
-      </c>
-      <c r="G9">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" t="e">
         <f t="shared" si="0"/>
-        <v>0.65522388059701486</v>
-      </c>
-      <c r="H9">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" t="e">
         <f t="shared" si="1"/>
-        <v>0.94612068965517238</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="55.2" thickBot="1" x14ac:dyDescent="0.65">
@@ -7265,25 +7127,17 @@
       <c r="B10" s="10">
         <v>1254501</v>
       </c>
-      <c r="C10" s="9">
-        <v>68</v>
-      </c>
-      <c r="D10" s="9">
-        <v>62</v>
-      </c>
-      <c r="E10" s="9">
-        <v>51.4</v>
-      </c>
-      <c r="F10" s="9">
-        <v>60</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" t="e">
         <f t="shared" si="0"/>
-        <v>0.75588235294117645</v>
-      </c>
-      <c r="H10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" t="e">
         <f t="shared" si="1"/>
-        <v>0.85666666666666669</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="73.2" x14ac:dyDescent="0.6">
@@ -7293,25 +7147,17 @@
       <c r="B11" s="24">
         <v>1505001</v>
       </c>
-      <c r="C11" s="17">
-        <v>76</v>
-      </c>
-      <c r="D11" s="17">
-        <v>71</v>
-      </c>
-      <c r="E11" s="17">
-        <v>60</v>
-      </c>
-      <c r="F11" s="17">
-        <v>64</v>
-      </c>
-      <c r="G11">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" t="e">
         <f t="shared" si="0"/>
-        <v>0.78947368421052633</v>
-      </c>
-      <c r="H11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" t="e">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -7342,7 +7188,7 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -7375,7 +7221,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7384,28 +7230,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -7597,14 +7443,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30C1AFB-536F-43E0-B3C1-1A8567A80FBF}">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31F4A23-90D7-46F5-AE97-C69CB8D96318}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="2" max="2" width="11.546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
@@ -7614,7 +7463,7 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -7647,7 +7496,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7656,28 +7505,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="27" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -7690,17 +7539,25 @@
       <c r="B8" s="19">
         <v>8070</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" t="e">
+      <c r="C8" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>116</v>
+      </c>
+      <c r="E8" s="4">
+        <v>96</v>
+      </c>
+      <c r="F8" s="4">
+        <v>35.1</v>
+      </c>
+      <c r="G8">
         <f>E8/C8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" t="e">
+        <v>2.3132530120481927</v>
+      </c>
+      <c r="H8">
         <f>E8/F8</f>
-        <v>#DIV/0!</v>
+        <v>2.7350427350427351</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
@@ -7710,17 +7567,25 @@
       <c r="B9" s="6">
         <v>42310</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" t="e">
-        <f t="shared" ref="G9:G12" si="0">E9/C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" t="e">
-        <f t="shared" ref="H9:H12" si="1">E9/F9</f>
-        <v>#DIV/0!</v>
+      <c r="C9" s="5">
+        <v>41.2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>115</v>
+      </c>
+      <c r="E9" s="5">
+        <v>96</v>
+      </c>
+      <c r="F9" s="5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G14" si="0">E9/C9</f>
+        <v>2.3300970873786406</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H14" si="1">E9/F9</f>
+        <v>2.7195467422096318</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -7730,17 +7595,25 @@
       <c r="B10" s="8">
         <v>89610</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" t="e">
+      <c r="C10" s="7">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D10" s="7">
+        <v>130</v>
+      </c>
+      <c r="E10" s="7">
+        <v>94</v>
+      </c>
+      <c r="F10" s="7">
+        <v>35.9</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" t="e">
+        <v>2.3918575063613234</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.6183844011142061</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
@@ -7750,17 +7623,25 @@
       <c r="B11" s="6">
         <v>648010</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" t="e">
+      <c r="C11" s="5">
+        <v>42.6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>121</v>
+      </c>
+      <c r="E11" s="5">
+        <v>98</v>
+      </c>
+      <c r="F11" s="5">
+        <v>35.9</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" t="e">
+        <v>2.300469483568075</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.7298050139275767</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
@@ -7770,17 +7651,25 @@
       <c r="B12" s="22">
         <v>1047210</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" t="e">
+      <c r="C12" s="23">
+        <v>48.4</v>
+      </c>
+      <c r="D12" s="23">
+        <v>118</v>
+      </c>
+      <c r="E12" s="23">
+        <v>99</v>
+      </c>
+      <c r="F12" s="23">
+        <v>36.4</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="20" t="e">
+        <v>2.0454545454545454</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2.7197802197802199</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7790,26 +7679,53 @@
       <c r="B13" s="10">
         <v>1796010</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" t="e">
-        <f>E13/C13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" t="e">
-        <f>E13/F13</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
-      <c r="A14" s="17"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
+      <c r="C13" s="9">
+        <v>65</v>
+      </c>
+      <c r="D13" s="9">
+        <v>128</v>
+      </c>
+      <c r="E13" s="9">
+        <v>98</v>
+      </c>
+      <c r="F13" s="9">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.5076923076923077</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.4078624078624076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="8">
+        <v>19184010</v>
+      </c>
+      <c r="C14" s="7">
+        <v>136</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7821,6 +7737,300 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30C1AFB-536F-43E0-B3C1-1A8567A80FBF}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="2" max="2" width="11.546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="19">
+        <v>8070</v>
+      </c>
+      <c r="C8" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>116</v>
+      </c>
+      <c r="E8" s="4">
+        <v>96</v>
+      </c>
+      <c r="F8" s="4">
+        <v>35.1</v>
+      </c>
+      <c r="G8">
+        <f>E8/C8</f>
+        <v>2.3132530120481927</v>
+      </c>
+      <c r="H8">
+        <f>E8/F8</f>
+        <v>2.7350427350427351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6">
+        <v>42310</v>
+      </c>
+      <c r="C9" s="5">
+        <v>41.2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>115</v>
+      </c>
+      <c r="E9" s="5">
+        <v>96</v>
+      </c>
+      <c r="F9" s="5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G14" si="0">E9/C9</f>
+        <v>2.3300970873786406</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H14" si="1">E9/F9</f>
+        <v>2.7195467422096318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8">
+        <v>89610</v>
+      </c>
+      <c r="C10" s="7">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D10" s="7">
+        <v>130</v>
+      </c>
+      <c r="E10" s="7">
+        <v>94</v>
+      </c>
+      <c r="F10" s="7">
+        <v>35.9</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2.3918575063613234</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.6183844011142061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6">
+        <v>648010</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42.6</v>
+      </c>
+      <c r="D11" s="5">
+        <v>121</v>
+      </c>
+      <c r="E11" s="5">
+        <v>98</v>
+      </c>
+      <c r="F11" s="5">
+        <v>35.9</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.300469483568075</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2.7298050139275767</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
+      <c r="A12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1047210</v>
+      </c>
+      <c r="C12" s="23">
+        <v>48.4</v>
+      </c>
+      <c r="D12" s="23">
+        <v>118</v>
+      </c>
+      <c r="E12" s="23">
+        <v>99</v>
+      </c>
+      <c r="F12" s="23">
+        <v>36.4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.0454545454545454</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>2.7197802197802199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="36.9" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1796010</v>
+      </c>
+      <c r="C13" s="9">
+        <v>65</v>
+      </c>
+      <c r="D13" s="9">
+        <v>128</v>
+      </c>
+      <c r="E13" s="9">
+        <v>98</v>
+      </c>
+      <c r="F13" s="9">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.5076923076923077</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.4078624078624076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="36.6" x14ac:dyDescent="0.6">
+      <c r="A14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="8">
+        <v>19184010</v>
+      </c>
+      <c r="C14" s="7">
+        <v>136</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55B451C-30A0-2146-8D94-EFD11E3F197D}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -7838,7 +8048,7 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -7871,7 +8081,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7880,28 +8090,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -8092,7 +8302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7FA1CC5-7431-4E08-8B84-CED1C73BE227}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -8152,10 +8362,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.3" x14ac:dyDescent="0.6">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -8172,8 +8382,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="2">
         <v>7</v>
       </c>

</xml_diff>